<commit_message>
chart moved to a different sheet
</commit_message>
<xml_diff>
--- a/resources/Salary.xlsx
+++ b/resources/Salary.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16927"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Palash\OneDrive\Office Sync\Tax Bill\Tax Bill - 2015-16\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="7410"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="7410" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Details" sheetId="1" r:id="rId1"/>
     <sheet name="Anum" sheetId="2" r:id="rId2"/>
+    <sheet name="Charts" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171026"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -87,10 +83,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="[$-14009]dd/mm/yyyy;@"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -137,7 +133,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -147,8 +143,8 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -171,18 +167,8 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -210,7 +196,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -218,33 +204,11 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -280,8 +244,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DF3D-49F8-8C0F-BB8577D0ADA9}"/>
             </c:ext>
@@ -322,34 +285,23 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-DF3D-49F8-8C0F-BB8577D0ADA9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="1369084808"/>
-        <c:axId val="1369086600"/>
+        <c:marker val="1"/>
+        <c:axId val="66228992"/>
+        <c:axId val="66230528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1369084808"/>
+        <c:axId val="66228992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
         <c:spPr>
           <a:noFill/>
@@ -384,15 +336,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1369086600"/>
+        <c:crossAx val="66230528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1369086600"/>
+        <c:axId val="66230528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,9 +379,8 @@
         </c:minorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1369084808"/>
+        <c:crossAx val="66228992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -444,7 +394,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:overlay val="0"/>
+      <c:layout/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -475,7 +425,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -504,589 +453,33 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 1">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3917B460-89E9-448A-BCF5-447C4E090ED2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3917B460-89E9-448A-BCF5-447C4E090ED2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1150,7 +543,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1202,7 +595,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1396,17 +789,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1757,7 +1150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1783,6 +1176,20 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>